<commit_message>
added best solution to problem
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -378,7 +378,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <f>SUM(B2:B16)</f>
@@ -442,9 +442,12 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="F3">
-        <f>D2/F2</f>
-        <v>3.3519553072625698E-2</v>
+        <f>SUM(D2:D16)/F2</f>
+        <v>6.1452513966480445E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -456,6 +459,9 @@
       </c>
       <c r="C4" t="s">
         <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -468,6 +474,9 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -479,6 +488,9 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -490,6 +502,9 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -500,6 +515,9 @@
       </c>
       <c r="C8" t="s">
         <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finsihed 6 problems in ch 6
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -378,7 +378,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,11 +446,11 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <f>SUM(D2:D16)/F2</f>
-        <v>0.15083798882681565</v>
+        <v>0.17318435754189945</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished 5 questions in ch5
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Chapters</t>
   </si>
@@ -37,6 +37,27 @@
   </si>
   <si>
     <t>Progress</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Linked L</t>
+  </si>
+  <si>
+    <t>Stacks</t>
+  </si>
+  <si>
+    <t>Binary T</t>
   </si>
 </sst>
 </file>
@@ -375,18 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,22 +415,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -417,25 +441,28 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>11</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <f>SUM(B2:B17)</f>
         <v>189</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <f>SUM(B18:B21)</f>
         <v>52</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <f>B22</f>
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -443,17 +470,20 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3">
-        <f>SUM(D2:D17)/F2</f>
-        <v>0.29629629629629628</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>SUM(E2:E17)/G2</f>
+        <v>0.32275132275132273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -461,13 +491,16 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -475,212 +508,234 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <f>A5+1</f>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f>F2/2</f>
-        <v>94.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <f t="shared" ref="A7:A22" si="0">A6+1</f>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>12</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished fizing queue library implementation, and max api implementation
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.32275132275132273</v>
+        <v>0.34920634920634919</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished ch 6 5th question
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.34920634920634919</v>
+        <v>0.35449735449735448</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished 5 questions in chapter 6
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.35449735449735448</v>
+        <v>0.40740740740740738</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -550,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished 4 questions in chapter 8
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.47619047619047616</v>
+        <v>0.50793650793650791</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished 5 questions in chapter 9
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.51851851851851849</v>
+        <v>0.58730158730158732</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -605,6 +605,9 @@
       </c>
       <c r="D10" t="s">
         <v>3</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished 2 questions in ch 9 with better than book answer
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="12090"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="12285" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -405,7 +406,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +487,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.58730158730158732</v>
+        <v>0.59788359788359791</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -607,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -763,7 +764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Finished 5 questions in chapter 11
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.65608465608465605</v>
+        <v>0.69841269841269837</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
almost finished chapter 11
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.69841269841269837</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished several problems in the recursive chapter
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="G3">
         <f>SUM(E2:E17)/G2</f>
-        <v>0.7142857142857143</v>
+        <v>0.7407407407407407</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>